<commit_message>
Bug fixes, updated test cases, presentation prep
</commit_message>
<xml_diff>
--- a/Phase 3 Documentation/Phase Three Time Log.xlsx
+++ b/Phase 3 Documentation/Phase Three Time Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeman/Documents/macos/Planr/Phase 3 Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61212ECE-DDF4-1D46-BB14-93BD1E9203A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B868C15-D21D-0646-A1AA-2499075B481F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
+    <workbookView xWindow="-28940" yWindow="1220" windowWidth="26600" windowHeight="17940" xr2:uid="{52085EF4-1DF1-914B-8651-54C060764F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -115,15 +115,34 @@
   </si>
   <si>
     <t>Testing the application and resolving bugs found</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Adding new test cases now that UI is more finalized.</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Documenting the new architecture changes.</t>
+  </si>
+  <si>
+    <t>Finalizing work on the presentation.</t>
+  </si>
+  <si>
+    <t>Code clean up and documentation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -162,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -175,6 +194,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,14 +513,14 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="103.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
@@ -554,7 +575,7 @@
         <v>0.9375</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D20" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D22" si="0">C3-B3</f>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E3" t="s">
@@ -848,11 +869,11 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="C18" s="3">
-        <v>24</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>23.041666666666668</v>
+        <v>4.0972222222222188E-2</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -901,22 +922,90 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.44375000000000003</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7916666666666718E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D34" s="5"/>
     </row>
   </sheetData>

</xml_diff>